<commit_message>
Flower and Fruit update
</commit_message>
<xml_diff>
--- a/data/Flower and Fruit numbers.xlsx
+++ b/data/Flower and Fruit numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c54973fbc0cfccc5/Documents/Harvard/Holbrook Labs/DaRin Butz/Phenophases-DRB/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\DaRin Butz Interns\Erin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="114_{EDAFF8BB-7B6B-45BC-91EA-60AD8CFDCCA9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{EDCF02BC-11D9-4BF1-86E5-9A2BB568CD34}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{531E74EE-DA88-4DAA-AC2E-4454C8490F7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{B9543983-0637-4653-AF61-5EE7608192B4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{B9543983-0637-4653-AF61-5EE7608192B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flower Data 2019" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="207">
   <si>
     <t>Plant ID Tag</t>
   </si>
@@ -653,17 +647,14 @@
     <t>SAMRAC_HF</t>
   </si>
   <si>
-    <t>SPIALB_SH_4B</t>
-  </si>
-  <si>
-    <t>SPIALB_HF_4</t>
+    <t>Harvard Forest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +664,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -695,16 +693,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1016,83 +1017,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ECA217-E551-457B-80A7-B3779EDD5783}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.9296875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.9296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.53125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.86328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43626</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43626</v>
       </c>
@@ -1152,6 +1153,9 @@
       <c r="C3" t="s">
         <v>157</v>
       </c>
+      <c r="E3" t="s">
+        <v>190</v>
+      </c>
       <c r="F3" t="s">
         <v>175</v>
       </c>
@@ -1189,7 +1193,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43626</v>
       </c>
@@ -1242,7 +1246,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43627</v>
       </c>
@@ -1252,6 +1256,9 @@
       <c r="C5" t="s">
         <v>183</v>
       </c>
+      <c r="E5" t="s">
+        <v>173</v>
+      </c>
       <c r="F5" t="s">
         <v>175</v>
       </c>
@@ -1289,7 +1296,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43627</v>
       </c>
@@ -1339,7 +1346,7 @@
         <v>157.6</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43622</v>
       </c>
@@ -1386,7 +1393,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43622</v>
       </c>
@@ -1436,7 +1443,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43630</v>
       </c>
@@ -1480,7 +1487,7 @@
         <v>148.1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43630</v>
       </c>
@@ -1530,7 +1537,7 @@
         <v>148.1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43630</v>
       </c>
@@ -1580,7 +1587,7 @@
         <v>148.1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43630</v>
       </c>
@@ -1630,7 +1637,7 @@
         <v>148.1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43630</v>
       </c>
@@ -1680,7 +1687,7 @@
         <v>63.3</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43630</v>
       </c>
@@ -1730,7 +1737,7 @@
         <v>158.1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43630</v>
       </c>
@@ -1774,7 +1781,7 @@
         <v>158.1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43630</v>
       </c>
@@ -1824,7 +1831,7 @@
         <v>158.1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43630</v>
       </c>
@@ -1868,7 +1875,7 @@
         <v>158.1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43630</v>
       </c>
@@ -1918,7 +1925,7 @@
         <v>193.2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43630</v>
       </c>
@@ -1968,7 +1975,7 @@
         <v>193.2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43630</v>
       </c>
@@ -2016,6 +2023,734 @@
       </c>
       <c r="P20">
         <v>193.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B21" s="2">
+        <v>172</v>
+      </c>
+      <c r="C21" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" t="s">
+        <v>175</v>
+      </c>
+      <c r="G21" t="s">
+        <v>176</v>
+      </c>
+      <c r="H21">
+        <f>0.04/5</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I21">
+        <f>0.007/5</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="J21">
+        <v>4.3049999999999997</v>
+      </c>
+      <c r="K21">
+        <v>4.2919999999999998</v>
+      </c>
+      <c r="L21" t="s">
+        <v>177</v>
+      </c>
+      <c r="M21" t="s">
+        <v>206</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B22" s="2">
+        <v>172</v>
+      </c>
+      <c r="C22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>172</v>
+      </c>
+      <c r="F22" t="s">
+        <v>175</v>
+      </c>
+      <c r="G22" t="s">
+        <v>176</v>
+      </c>
+      <c r="H22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I22">
+        <v>1.4E-3</v>
+      </c>
+      <c r="J22">
+        <v>3.01</v>
+      </c>
+      <c r="K22">
+        <v>2.4780000000000002</v>
+      </c>
+      <c r="L22" t="s">
+        <v>177</v>
+      </c>
+      <c r="M22" t="s">
+        <v>206</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B23" s="2">
+        <v>172</v>
+      </c>
+      <c r="C23" t="s">
+        <v>205</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>172</v>
+      </c>
+      <c r="F23" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" t="s">
+        <v>176</v>
+      </c>
+      <c r="H23">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I23">
+        <v>1.4E-3</v>
+      </c>
+      <c r="J23">
+        <v>3.7109999999999999</v>
+      </c>
+      <c r="K23">
+        <v>0.29730000000000001</v>
+      </c>
+      <c r="L23" t="s">
+        <v>177</v>
+      </c>
+      <c r="M23" t="s">
+        <v>206</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B24" s="2">
+        <v>172</v>
+      </c>
+      <c r="C24" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>172</v>
+      </c>
+      <c r="F24" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" t="s">
+        <v>176</v>
+      </c>
+      <c r="H24">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I24">
+        <v>1.4E-3</v>
+      </c>
+      <c r="J24">
+        <v>3.629</v>
+      </c>
+      <c r="K24">
+        <v>3.4169999999999998</v>
+      </c>
+      <c r="L24" t="s">
+        <v>177</v>
+      </c>
+      <c r="M24" t="s">
+        <v>206</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B25" s="2">
+        <v>172</v>
+      </c>
+      <c r="C25" t="s">
+        <v>205</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>172</v>
+      </c>
+      <c r="F25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H25">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I25">
+        <v>1.4E-3</v>
+      </c>
+      <c r="J25">
+        <v>4.1310000000000002</v>
+      </c>
+      <c r="K25">
+        <v>3.3780000000000001</v>
+      </c>
+      <c r="L25" t="s">
+        <v>177</v>
+      </c>
+      <c r="M25" t="s">
+        <v>206</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B26" s="2">
+        <v>172</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>172</v>
+      </c>
+      <c r="F26" t="s">
+        <v>175</v>
+      </c>
+      <c r="G26" t="s">
+        <v>176</v>
+      </c>
+      <c r="H26">
+        <f>0.058/6</f>
+        <v>9.6666666666666672E-3</v>
+      </c>
+      <c r="I26">
+        <f>0.011/6</f>
+        <v>1.8333333333333333E-3</v>
+      </c>
+      <c r="J26">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K26">
+        <v>4.0289999999999999</v>
+      </c>
+      <c r="L26" t="s">
+        <v>177</v>
+      </c>
+      <c r="M26" t="s">
+        <v>206</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B27" s="2">
+        <v>172</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" t="s">
+        <v>175</v>
+      </c>
+      <c r="G27" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27:H31" si="0">0.058/6</f>
+        <v>9.6666666666666672E-3</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27:I31" si="1">0.011/6</f>
+        <v>1.8333333333333333E-3</v>
+      </c>
+      <c r="J27">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="K27">
+        <v>4.2110000000000003</v>
+      </c>
+      <c r="L27" t="s">
+        <v>177</v>
+      </c>
+      <c r="M27" t="s">
+        <v>206</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B28" s="2">
+        <v>172</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>172</v>
+      </c>
+      <c r="F28" t="s">
+        <v>175</v>
+      </c>
+      <c r="G28" t="s">
+        <v>176</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666672E-3</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>1.8333333333333333E-3</v>
+      </c>
+      <c r="J28">
+        <v>3.9380000000000002</v>
+      </c>
+      <c r="K28">
+        <v>4.359</v>
+      </c>
+      <c r="L28" t="s">
+        <v>177</v>
+      </c>
+      <c r="M28" t="s">
+        <v>206</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B29" s="2">
+        <v>172</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>172</v>
+      </c>
+      <c r="F29" t="s">
+        <v>175</v>
+      </c>
+      <c r="G29" t="s">
+        <v>176</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666672E-3</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>1.8333333333333333E-3</v>
+      </c>
+      <c r="J29">
+        <v>3.68</v>
+      </c>
+      <c r="K29">
+        <v>4.077</v>
+      </c>
+      <c r="L29" t="s">
+        <v>177</v>
+      </c>
+      <c r="M29" t="s">
+        <v>206</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B30" s="2">
+        <v>172</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>172</v>
+      </c>
+      <c r="F30" t="s">
+        <v>175</v>
+      </c>
+      <c r="G30" t="s">
+        <v>176</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666672E-3</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>1.8333333333333333E-3</v>
+      </c>
+      <c r="J30">
+        <v>4.03</v>
+      </c>
+      <c r="K30">
+        <v>4.1449999999999996</v>
+      </c>
+      <c r="L30" t="s">
+        <v>177</v>
+      </c>
+      <c r="M30" t="s">
+        <v>206</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B31" s="2">
+        <v>172</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>172</v>
+      </c>
+      <c r="F31" t="s">
+        <v>175</v>
+      </c>
+      <c r="G31" t="s">
+        <v>176</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666672E-3</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>1.8333333333333333E-3</v>
+      </c>
+      <c r="J31">
+        <v>3.9350000000000001</v>
+      </c>
+      <c r="K31">
+        <v>4.0490000000000004</v>
+      </c>
+      <c r="L31" t="s">
+        <v>177</v>
+      </c>
+      <c r="M31" t="s">
+        <v>206</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B32" s="2">
+        <v>172</v>
+      </c>
+      <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>172</v>
+      </c>
+      <c r="F32" t="s">
+        <v>175</v>
+      </c>
+      <c r="G32" t="s">
+        <v>176</v>
+      </c>
+      <c r="H32">
+        <f>0.036/5</f>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="I32">
+        <f>0.007/5</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="J32">
+        <v>3.883</v>
+      </c>
+      <c r="K32">
+        <v>3.81</v>
+      </c>
+      <c r="L32" t="s">
+        <v>177</v>
+      </c>
+      <c r="M32" t="s">
+        <v>206</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B33" s="2">
+        <v>172</v>
+      </c>
+      <c r="C33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>172</v>
+      </c>
+      <c r="F33" t="s">
+        <v>175</v>
+      </c>
+      <c r="G33" t="s">
+        <v>176</v>
+      </c>
+      <c r="H33">
+        <f t="shared" ref="H33:H36" si="2">0.036/5</f>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ref="I33:I36" si="3">0.007/5</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="J33">
+        <v>3.7610000000000001</v>
+      </c>
+      <c r="K33">
+        <v>3.9449999999999998</v>
+      </c>
+      <c r="L33" t="s">
+        <v>177</v>
+      </c>
+      <c r="M33" t="s">
+        <v>206</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B34" s="2">
+        <v>172</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>172</v>
+      </c>
+      <c r="F34" t="s">
+        <v>175</v>
+      </c>
+      <c r="G34" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="3"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="J34">
+        <v>2.8780000000000001</v>
+      </c>
+      <c r="K34">
+        <v>4.0339999999999998</v>
+      </c>
+      <c r="L34" t="s">
+        <v>177</v>
+      </c>
+      <c r="M34" t="s">
+        <v>206</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B35" s="2">
+        <v>172</v>
+      </c>
+      <c r="C35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35" t="s">
+        <v>172</v>
+      </c>
+      <c r="F35" t="s">
+        <v>175</v>
+      </c>
+      <c r="G35" t="s">
+        <v>176</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="3"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="J35">
+        <v>3.0539999999999998</v>
+      </c>
+      <c r="K35">
+        <v>4.0090000000000003</v>
+      </c>
+      <c r="L35" t="s">
+        <v>177</v>
+      </c>
+      <c r="M35" t="s">
+        <v>206</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B36" s="2">
+        <v>172</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>172</v>
+      </c>
+      <c r="F36" t="s">
+        <v>175</v>
+      </c>
+      <c r="G36" t="s">
+        <v>176</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="J36">
+        <v>2.653</v>
+      </c>
+      <c r="K36">
+        <v>3.4470000000000001</v>
+      </c>
+      <c r="L36" t="s">
+        <v>177</v>
+      </c>
+      <c r="M36" t="s">
+        <v>206</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2025,34 +2760,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0040E16A-6A45-4C34-B5DE-8934C713DD5F}">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.53125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2105,7 +2840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43633</v>
       </c>
@@ -2143,7 +2878,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43633</v>
       </c>
@@ -2181,7 +2916,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43633</v>
       </c>
@@ -2219,7 +2954,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43633</v>
       </c>
@@ -2257,7 +2992,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43633</v>
       </c>
@@ -2295,7 +3030,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43633</v>
       </c>
@@ -2333,7 +3068,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43633</v>
       </c>
@@ -2371,7 +3106,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43633</v>
       </c>
@@ -2409,7 +3144,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43633</v>
       </c>
@@ -2447,7 +3182,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43633</v>
       </c>
@@ -2485,7 +3220,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43633</v>
       </c>
@@ -2523,7 +3258,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43633</v>
       </c>
@@ -2561,7 +3296,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43633</v>
       </c>
@@ -2599,7 +3334,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43633</v>
       </c>
@@ -2637,7 +3372,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43633</v>
       </c>
@@ -2675,7 +3410,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43633</v>
       </c>
@@ -2713,7 +3448,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43633</v>
       </c>
@@ -2751,7 +3486,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43633</v>
       </c>
@@ -2789,7 +3524,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43633</v>
       </c>
@@ -2827,7 +3562,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43633</v>
       </c>
@@ -2865,7 +3600,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43633</v>
       </c>
@@ -2903,7 +3638,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43633</v>
       </c>
@@ -2941,7 +3676,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43633</v>
       </c>
@@ -2979,7 +3714,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43633</v>
       </c>
@@ -3017,7 +3752,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43633</v>
       </c>
@@ -3055,7 +3790,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43633</v>
       </c>
@@ -3093,7 +3828,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43633</v>
       </c>
@@ -3118,6 +3853,12 @@
       <c r="H28">
         <v>3.1E-2</v>
       </c>
+      <c r="I28">
+        <v>2.4590000000000001</v>
+      </c>
+      <c r="J28">
+        <v>2.23</v>
+      </c>
       <c r="N28" t="s">
         <v>195</v>
       </c>
@@ -3125,7 +3866,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43633</v>
       </c>
@@ -3150,6 +3891,12 @@
       <c r="H29">
         <v>2.9000000000000001E-2</v>
       </c>
+      <c r="I29">
+        <v>2.6480000000000001</v>
+      </c>
+      <c r="J29">
+        <v>2.399</v>
+      </c>
       <c r="N29" t="s">
         <v>195</v>
       </c>
@@ -3157,7 +3904,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43633</v>
       </c>
@@ -3182,6 +3929,12 @@
       <c r="H30">
         <v>4.1000000000000002E-2</v>
       </c>
+      <c r="I30">
+        <v>2.5249999999999999</v>
+      </c>
+      <c r="J30">
+        <v>2.476</v>
+      </c>
       <c r="N30" t="s">
         <v>195</v>
       </c>
@@ -3189,349 +3942,14 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A31" s="1">
-        <v>43637</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>193</v>
-      </c>
-      <c r="F31" t="s">
-        <v>176</v>
-      </c>
-      <c r="G31">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="H31">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>193</v>
-      </c>
-      <c r="F36" t="s">
-        <v>176</v>
-      </c>
-      <c r="G36">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="H36">
-        <v>5.8000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C41" t="s">
-        <v>70</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D44">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C46" t="s">
-        <v>183</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="D48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D49">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C51" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D54">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D55">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A56" s="1">
-        <v>43630</v>
-      </c>
-      <c r="C56" t="s">
-        <v>97</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D58">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D59">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D60">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A61" s="1">
-        <v>43637</v>
-      </c>
-      <c r="C61" t="s">
-        <v>68</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D62">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D64">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D65">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C66" t="s">
-        <v>205</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D68">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D69">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D70">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C71" t="s">
-        <v>206</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D73">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D74">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D75">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C76" t="s">
-        <v>72</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D78">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D80">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C81" t="s">
-        <v>207</v>
-      </c>
-      <c r="D81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D82">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D83">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D84">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D85">
-        <v>5</v>
-      </c>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3547,14 +3965,14 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3565,7 +3983,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3573,7 +3991,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3581,7 +3999,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -3589,7 +4007,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -3597,7 +4015,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -3605,7 +4023,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3613,7 +4031,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3621,7 +4039,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3629,7 +4047,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -3637,7 +4055,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -3645,7 +4063,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -3653,7 +4071,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -3661,7 +4079,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -3669,7 +4087,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -3677,7 +4095,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3685,7 +4103,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -3693,7 +4111,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -3701,7 +4119,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -3709,7 +4127,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -3717,7 +4135,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -3725,7 +4143,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -3733,7 +4151,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -3741,7 +4159,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -3749,7 +4167,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3757,7 +4175,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -3765,7 +4183,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -3773,7 +4191,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -3781,7 +4199,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -3789,7 +4207,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -3797,7 +4215,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -3805,7 +4223,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -3813,7 +4231,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -3821,7 +4239,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -3829,7 +4247,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -3837,7 +4255,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -3845,7 +4263,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -3853,7 +4271,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -3861,7 +4279,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -3869,7 +4287,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -3877,7 +4295,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -3885,7 +4303,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -3893,7 +4311,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -3901,7 +4319,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -3909,7 +4327,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>61</v>
       </c>
@@ -3917,7 +4335,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -3925,7 +4343,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -3933,7 +4351,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -3941,7 +4359,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -3949,7 +4367,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>65</v>
       </c>
@@ -3957,7 +4375,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -3965,7 +4383,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -3973,7 +4391,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -3981,7 +4399,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>69</v>
       </c>
@@ -3989,7 +4407,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -3997,7 +4415,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -4005,7 +4423,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -4013,7 +4431,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -4021,7 +4439,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -4029,7 +4447,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -4037,7 +4455,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -4045,7 +4463,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -4053,7 +4471,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -4061,7 +4479,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -4069,7 +4487,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>81</v>
       </c>
@@ -4077,7 +4495,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -4085,7 +4503,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -4093,7 +4511,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -4101,7 +4519,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -4109,7 +4527,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -4117,7 +4535,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>89</v>
       </c>
@@ -4125,7 +4543,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -4133,7 +4551,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>91</v>
       </c>
@@ -4141,7 +4559,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -4149,7 +4567,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -4157,7 +4575,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -4165,7 +4583,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>92</v>
       </c>
@@ -4173,7 +4591,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>93</v>
       </c>
@@ -4181,7 +4599,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>94</v>
       </c>
@@ -4189,7 +4607,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>95</v>
       </c>
@@ -4197,7 +4615,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>96</v>
       </c>
@@ -4205,7 +4623,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>97</v>
       </c>
@@ -4213,7 +4631,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>98</v>
       </c>
@@ -4221,7 +4639,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>99</v>
       </c>
@@ -4229,7 +4647,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>100</v>
       </c>
@@ -4237,7 +4655,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -4245,7 +4663,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>102</v>
       </c>
@@ -4253,7 +4671,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>103</v>
       </c>
@@ -4261,7 +4679,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>104</v>
       </c>
@@ -4269,7 +4687,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>105</v>
       </c>
@@ -4277,7 +4695,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>106</v>
       </c>
@@ -4285,7 +4703,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>109</v>
       </c>
@@ -4293,7 +4711,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -4301,7 +4719,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>108</v>
       </c>
@@ -4309,7 +4727,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -4317,7 +4735,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>111</v>
       </c>
@@ -4325,7 +4743,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>112</v>
       </c>
@@ -4333,7 +4751,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>113</v>
       </c>
@@ -4341,7 +4759,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -4349,7 +4767,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>115</v>
       </c>
@@ -4357,7 +4775,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>116</v>
       </c>
@@ -4365,7 +4783,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>117</v>
       </c>
@@ -4373,7 +4791,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>118</v>
       </c>
@@ -4381,7 +4799,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>119</v>
       </c>
@@ -4389,7 +4807,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>120</v>
       </c>
@@ -4397,7 +4815,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>121</v>
       </c>
@@ -4405,7 +4823,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>122</v>
       </c>
@@ -4413,7 +4831,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>123</v>
       </c>
@@ -4421,7 +4839,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>124</v>
       </c>
@@ -4429,7 +4847,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>125</v>
       </c>
@@ -4437,7 +4855,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>126</v>
       </c>
@@ -4445,7 +4863,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>127</v>
       </c>
@@ -4453,7 +4871,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>128</v>
       </c>
@@ -4461,7 +4879,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>129</v>
       </c>
@@ -4469,7 +4887,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -4477,7 +4895,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>131</v>
       </c>
@@ -4485,7 +4903,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>132</v>
       </c>
@@ -4493,7 +4911,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>133</v>
       </c>
@@ -4501,7 +4919,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>134</v>
       </c>
@@ -4509,7 +4927,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>135</v>
       </c>
@@ -4517,7 +4935,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>136</v>
       </c>
@@ -4525,7 +4943,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>137</v>
       </c>
@@ -4533,7 +4951,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>138</v>
       </c>
@@ -4541,7 +4959,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>139</v>
       </c>
@@ -4549,7 +4967,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>140</v>
       </c>
@@ -4557,7 +4975,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>141</v>
       </c>
@@ -4565,7 +4983,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>143</v>
       </c>
@@ -4573,7 +4991,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -4581,7 +4999,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>144</v>
       </c>
@@ -4589,7 +5007,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>145</v>
       </c>
@@ -4597,7 +5015,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>146</v>
       </c>
@@ -4605,7 +5023,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>147</v>
       </c>
@@ -4613,7 +5031,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>148</v>
       </c>
@@ -4621,7 +5039,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>149</v>
       </c>
@@ -4629,7 +5047,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>150</v>
       </c>
@@ -4637,7 +5055,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>151</v>
       </c>
@@ -4645,7 +5063,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>152</v>
       </c>
@@ -4653,7 +5071,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>153</v>
       </c>
@@ -4661,7 +5079,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>154</v>
       </c>
@@ -4669,7 +5087,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>155</v>
       </c>
@@ -4677,7 +5095,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>156</v>
       </c>
@@ -4685,7 +5103,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>157</v>
       </c>
@@ -4693,7 +5111,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>158</v>
       </c>
@@ -4701,7 +5119,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>159</v>
       </c>
@@ -4709,7 +5127,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>160</v>
       </c>
@@ -4717,7 +5135,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>161</v>
       </c>
@@ -4725,7 +5143,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>162</v>
       </c>
@@ -4733,7 +5151,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>163</v>
       </c>
@@ -4741,7 +5159,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>164</v>
       </c>
@@ -4749,7 +5167,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>166</v>
       </c>
@@ -4757,7 +5175,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>165</v>
       </c>
@@ -4765,7 +5183,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>167</v>
       </c>
@@ -4773,7 +5191,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>168</v>
       </c>

</xml_diff>

<commit_message>
Update Flower and Fruit numbers.xlsx
</commit_message>
<xml_diff>
--- a/data/Flower and Fruit numbers.xlsx
+++ b/data/Flower and Fruit numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\DaRin Butz Interns\Erin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ubcwr\OneDrive\Documents\Harvard\Holbrook Labs\DaRin Butz\Phenophases-DRB\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{531E74EE-DA88-4DAA-AC2E-4454C8490F7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60B551F-FF5C-4912-905C-2053350E2BDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{B9543983-0637-4653-AF61-5EE7608192B4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{B9543983-0637-4653-AF61-5EE7608192B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flower Data 2019" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,12 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1019,31 +1025,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ECA217-E551-457B-80A7-B3779EDD5783}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.86328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1093,7 +1099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>43626</v>
       </c>
@@ -1143,7 +1149,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>43626</v>
       </c>
@@ -1193,7 +1199,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>43626</v>
       </c>
@@ -1246,7 +1252,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>43627</v>
       </c>
@@ -1296,7 +1302,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>43627</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>157.6</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>43622</v>
       </c>
@@ -1393,7 +1399,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>43622</v>
       </c>
@@ -1443,7 +1449,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>43630</v>
       </c>
@@ -1487,7 +1493,7 @@
         <v>148.1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>43630</v>
       </c>
@@ -1537,7 +1543,7 @@
         <v>148.1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>43630</v>
       </c>
@@ -1587,7 +1593,7 @@
         <v>148.1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>43630</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>148.1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>43630</v>
       </c>
@@ -1687,7 +1693,7 @@
         <v>63.3</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>43630</v>
       </c>
@@ -1737,7 +1743,7 @@
         <v>158.1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>43630</v>
       </c>
@@ -1781,7 +1787,7 @@
         <v>158.1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>43630</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>158.1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>43630</v>
       </c>
@@ -1875,7 +1881,7 @@
         <v>158.1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>43630</v>
       </c>
@@ -1925,7 +1931,7 @@
         <v>193.2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>43630</v>
       </c>
@@ -1975,7 +1981,7 @@
         <v>193.2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>43630</v>
       </c>
@@ -2025,7 +2031,7 @@
         <v>193.2</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>43637</v>
       </c>
@@ -2071,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>43637</v>
       </c>
@@ -2115,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>43637</v>
       </c>
@@ -2159,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>43637</v>
       </c>
@@ -2203,7 +2209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>43637</v>
       </c>
@@ -2247,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>43637</v>
       </c>
@@ -2293,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>43637</v>
       </c>
@@ -2339,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>43637</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>43637</v>
       </c>
@@ -2431,7 +2437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>43637</v>
       </c>
@@ -2477,7 +2483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>43637</v>
       </c>
@@ -2523,7 +2529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>43637</v>
       </c>
@@ -2569,7 +2575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>43637</v>
       </c>
@@ -2615,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>43637</v>
       </c>
@@ -2661,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>43637</v>
       </c>
@@ -2707,7 +2713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>43637</v>
       </c>
@@ -2766,28 +2772,28 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.86328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.86328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2840,7 +2846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>43633</v>
       </c>
@@ -2878,7 +2884,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>43633</v>
       </c>
@@ -2916,7 +2922,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>43633</v>
       </c>
@@ -2954,7 +2960,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>43633</v>
       </c>
@@ -2992,7 +2998,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>43633</v>
       </c>
@@ -3030,7 +3036,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>43633</v>
       </c>
@@ -3068,7 +3074,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>43633</v>
       </c>
@@ -3106,7 +3112,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>43633</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>43633</v>
       </c>
@@ -3182,7 +3188,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>43633</v>
       </c>
@@ -3220,7 +3226,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>43633</v>
       </c>
@@ -3258,7 +3264,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>43633</v>
       </c>
@@ -3296,7 +3302,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>43633</v>
       </c>
@@ -3334,7 +3340,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>43633</v>
       </c>
@@ -3372,7 +3378,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>43633</v>
       </c>
@@ -3410,7 +3416,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>43633</v>
       </c>
@@ -3448,7 +3454,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>43633</v>
       </c>
@@ -3486,7 +3492,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>43633</v>
       </c>
@@ -3524,7 +3530,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>43633</v>
       </c>
@@ -3562,7 +3568,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>43633</v>
       </c>
@@ -3600,7 +3606,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>43633</v>
       </c>
@@ -3638,7 +3644,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>43633</v>
       </c>
@@ -3676,7 +3682,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>43633</v>
       </c>
@@ -3714,7 +3720,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>43633</v>
       </c>
@@ -3752,7 +3758,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>43633</v>
       </c>
@@ -3790,7 +3796,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>43633</v>
       </c>
@@ -3828,7 +3834,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>43633</v>
       </c>
@@ -3866,7 +3872,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>43633</v>
       </c>
@@ -3904,7 +3910,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>43633</v>
       </c>
@@ -3942,13 +3948,13 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
     </row>
   </sheetData>
@@ -3961,18 +3967,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC3088F-649B-4866-B1FA-2D3E8C217B8C}">
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3983,7 +3989,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3991,7 +3997,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3999,7 +4005,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -4007,7 +4013,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -4015,7 +4021,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -4023,7 +4029,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4031,7 +4037,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -4039,7 +4045,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -4047,7 +4053,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -4055,7 +4061,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -4063,7 +4069,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -4071,7 +4077,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -4079,7 +4085,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -4087,7 +4093,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -4095,7 +4101,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -4103,7 +4109,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -4111,7 +4117,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -4119,7 +4125,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -4127,7 +4133,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -4135,7 +4141,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -4143,7 +4149,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -4151,7 +4157,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -4159,7 +4165,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -4167,7 +4173,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -4175,7 +4181,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -4183,7 +4189,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -4191,7 +4197,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -4199,7 +4205,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -4207,7 +4213,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -4215,7 +4221,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -4223,7 +4229,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -4231,7 +4237,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -4239,7 +4245,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -4247,7 +4253,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -4255,7 +4261,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -4263,7 +4269,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -4271,7 +4277,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -4279,7 +4285,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -4287,7 +4293,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -4295,7 +4301,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -4303,7 +4309,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -4311,7 +4317,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -4319,7 +4325,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -4327,7 +4333,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>61</v>
       </c>
@@ -4335,7 +4341,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -4343,7 +4349,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -4351,7 +4357,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -4359,7 +4365,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -4367,7 +4373,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>65</v>
       </c>
@@ -4375,7 +4381,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -4383,7 +4389,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -4391,7 +4397,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -4399,7 +4405,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>69</v>
       </c>
@@ -4407,7 +4413,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -4415,7 +4421,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -4423,7 +4429,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -4431,7 +4437,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -4439,7 +4445,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -4447,7 +4453,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -4455,7 +4461,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -4463,7 +4469,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -4471,7 +4477,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -4479,7 +4485,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -4487,7 +4493,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>81</v>
       </c>
@@ -4495,7 +4501,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -4503,7 +4509,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -4511,7 +4517,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -4519,7 +4525,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -4527,7 +4533,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -4535,7 +4541,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>89</v>
       </c>
@@ -4543,7 +4549,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -4551,7 +4557,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>91</v>
       </c>
@@ -4559,7 +4565,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -4567,7 +4573,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -4575,7 +4581,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -4583,7 +4589,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>92</v>
       </c>
@@ -4591,7 +4597,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>93</v>
       </c>
@@ -4599,7 +4605,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>94</v>
       </c>
@@ -4607,7 +4613,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>95</v>
       </c>
@@ -4615,7 +4621,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>96</v>
       </c>
@@ -4623,7 +4629,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>97</v>
       </c>
@@ -4631,7 +4637,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>98</v>
       </c>
@@ -4639,7 +4645,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>99</v>
       </c>
@@ -4647,7 +4653,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>100</v>
       </c>
@@ -4655,7 +4661,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -4663,7 +4669,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>102</v>
       </c>
@@ -4671,7 +4677,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>103</v>
       </c>
@@ -4679,7 +4685,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>104</v>
       </c>
@@ -4687,7 +4693,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>105</v>
       </c>
@@ -4695,7 +4701,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>106</v>
       </c>
@@ -4703,7 +4709,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>109</v>
       </c>
@@ -4711,7 +4717,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -4719,7 +4725,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>108</v>
       </c>
@@ -4727,7 +4733,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -4735,7 +4741,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>111</v>
       </c>
@@ -4743,7 +4749,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>112</v>
       </c>
@@ -4751,7 +4757,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>113</v>
       </c>
@@ -4759,7 +4765,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -4767,7 +4773,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>115</v>
       </c>
@@ -4775,7 +4781,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>116</v>
       </c>
@@ -4783,7 +4789,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>117</v>
       </c>
@@ -4791,7 +4797,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>118</v>
       </c>
@@ -4799,7 +4805,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>119</v>
       </c>
@@ -4807,7 +4813,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>120</v>
       </c>
@@ -4815,7 +4821,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>121</v>
       </c>
@@ -4823,7 +4829,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>122</v>
       </c>
@@ -4831,7 +4837,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>123</v>
       </c>
@@ -4839,7 +4845,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>124</v>
       </c>
@@ -4847,7 +4853,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>125</v>
       </c>
@@ -4855,7 +4861,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>126</v>
       </c>
@@ -4863,7 +4869,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>127</v>
       </c>
@@ -4871,7 +4877,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>128</v>
       </c>
@@ -4879,7 +4885,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>129</v>
       </c>
@@ -4887,7 +4893,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -4895,7 +4901,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>131</v>
       </c>
@@ -4903,7 +4909,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>132</v>
       </c>
@@ -4911,7 +4917,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>133</v>
       </c>
@@ -4919,7 +4925,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>134</v>
       </c>
@@ -4927,7 +4933,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>135</v>
       </c>
@@ -4935,7 +4941,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>136</v>
       </c>
@@ -4943,7 +4949,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>137</v>
       </c>
@@ -4951,7 +4957,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>138</v>
       </c>
@@ -4959,7 +4965,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>139</v>
       </c>
@@ -4967,7 +4973,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>140</v>
       </c>
@@ -4975,7 +4981,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>141</v>
       </c>
@@ -4983,7 +4989,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>143</v>
       </c>
@@ -4991,7 +4997,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -4999,7 +5005,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>144</v>
       </c>
@@ -5007,7 +5013,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>145</v>
       </c>
@@ -5015,7 +5021,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>146</v>
       </c>
@@ -5023,7 +5029,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>147</v>
       </c>
@@ -5031,7 +5037,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>148</v>
       </c>
@@ -5039,7 +5045,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>149</v>
       </c>
@@ -5047,7 +5053,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>150</v>
       </c>
@@ -5055,7 +5061,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>151</v>
       </c>
@@ -5063,7 +5069,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>152</v>
       </c>
@@ -5071,7 +5077,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>153</v>
       </c>
@@ -5079,7 +5085,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>154</v>
       </c>
@@ -5087,7 +5093,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>155</v>
       </c>
@@ -5095,7 +5101,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>156</v>
       </c>
@@ -5103,7 +5109,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>157</v>
       </c>
@@ -5111,7 +5117,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>158</v>
       </c>
@@ -5119,7 +5125,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>159</v>
       </c>
@@ -5127,7 +5133,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>160</v>
       </c>
@@ -5135,7 +5141,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>161</v>
       </c>
@@ -5143,7 +5149,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>162</v>
       </c>
@@ -5151,7 +5157,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>163</v>
       </c>
@@ -5159,7 +5165,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>164</v>
       </c>
@@ -5167,7 +5173,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>166</v>
       </c>
@@ -5175,7 +5181,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>165</v>
       </c>
@@ -5183,7 +5189,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>167</v>
       </c>
@@ -5191,7 +5197,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>168</v>
       </c>

</xml_diff>